<commit_message>
tasks affectation by hour done
</commit_message>
<xml_diff>
--- a/excel-file.xlsx
+++ b/excel-file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\affectation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCA9A6D-4F6A-434D-923E-7C0895B9F40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317F4EC1-2EE9-4861-A926-C460D00324A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B943C160-DD57-409F-B5A3-655CF21E0259}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
   <si>
     <t>type</t>
   </si>
   <si>
-    <t>difficulty</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -59,20 +56,53 @@
     <t>portabilité</t>
   </si>
   <si>
-    <t xml:space="preserve"> xx-xxxx-xx</t>
-  </si>
-  <si>
     <t>aa</t>
   </si>
   <si>
-    <t>start_date</t>
+    <t xml:space="preserve"> xx-ftth-xx</t>
+  </si>
+  <si>
+    <t>startDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heure </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 09:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 08:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 07:00:00</t>
+  </si>
+  <si>
+    <t>as-xxxx-xx</t>
+  </si>
+  <si>
+    <t>ot-xxxx-xx</t>
+  </si>
+  <si>
+    <t>xx-ftth-xx</t>
+  </si>
+  <si>
+    <t>xx-rsta-xx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +115,12 @@
       <color rgb="FFA31515"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,7 +148,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,13 +463,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28B00D5-F45F-4E8B-8CFA-72D6585E8D8F}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -446,7 +485,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>9</v>
@@ -454,158 +493,312 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2">
-        <v>45230</v>
+        <v>15</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2">
-        <v>45231</v>
+        <v>16</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2">
-        <v>45232</v>
+        <v>17</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2">
-        <v>45233</v>
+      <c r="D5" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2">
-        <v>45234</v>
+        <v>16</v>
+      </c>
+      <c r="D6" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2">
-        <v>45235</v>
+        <v>18</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2">
-        <v>45236</v>
+        <v>15</v>
+      </c>
+      <c r="D8" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2">
-        <v>45237</v>
+        <v>15</v>
+      </c>
+      <c r="D9" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2">
-        <v>45238</v>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="2">
+        <v>45232</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
affectation task works great
</commit_message>
<xml_diff>
--- a/excel-file.xlsx
+++ b/excel-file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\affectation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317F4EC1-2EE9-4861-A926-C460D00324A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F15C27-DBB6-4557-847F-89FA13729858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B943C160-DD57-409F-B5A3-655CF21E0259}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="14">
   <si>
     <t>type</t>
   </si>
@@ -66,21 +66,6 @@
   </si>
   <si>
     <t xml:space="preserve">heure </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 09:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 08:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 07:00:00</t>
   </si>
   <si>
     <t>as-xxxx-xx</t>
@@ -143,12 +128,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +452,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,13 +485,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
+        <v>45231</v>
+      </c>
+      <c r="E2" s="3">
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -516,13 +502,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
+        <v>45231</v>
+      </c>
+      <c r="E3" s="3">
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -533,13 +519,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
+        <v>45231</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.125</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -553,10 +539,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
+        <v>45231</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.16666666666666699</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -567,30 +553,30 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
+        <v>45231</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.20833333333333401</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
+        <v>45231</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -601,13 +587,13 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
+        <v>45231</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.29166666666666702</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -618,13 +604,13 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
+        <v>45231</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.33333333333333398</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -635,13 +621,13 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
+        <v>45231</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.375</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -652,13 +638,13 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
+        <v>45231</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.41666666666666702</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -669,30 +655,30 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
+        <v>45231</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.45833333333333398</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
+        <v>45231</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -703,13 +689,13 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
+        <v>45231</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.54166666666666696</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -720,30 +706,30 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
+        <v>45231</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.58333333333333404</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D16" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E16" t="s">
-        <v>10</v>
+        <v>45231</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.625</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -754,13 +740,13 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E17" t="s">
-        <v>10</v>
+        <v>45231</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.66666666666666696</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -771,13 +757,13 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D18" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
+        <v>45231</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.70833333333333404</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -788,13 +774,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D19" s="2">
-        <v>45232</v>
-      </c>
-      <c r="E19" t="s">
-        <v>12</v>
+        <v>45231</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>